<commit_message>
change regular expression methods
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t xml:space="preserve">title</t>
   </si>
@@ -49,16 +49,19 @@
     <t xml:space="preserve">keyword1, keyword2, keyword3</t>
   </si>
   <si>
+    <t xml:space="preserve">Dummy. Dummy. Dummy. Dummy. Dummy. &lt;i&gt;Dummy&lt;/i&gt;. Dummy. Dummy. &lt;i&gt;Dummy&lt;/i&gt;. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fugafuga method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hanako Todai(1), Taro Waseda(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1) The University of Tokyo, (2) Waseda University</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. Dummy. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">fugafuga method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hanako Todai(1), Taro Waseda(2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1) The University of Tokyo, (2) Waseda University</t>
   </si>
   <si>
     <t xml:space="preserve">Expanding hogefuga</t>
@@ -76,6 +79,7 @@
       <sz val="10"/>
       <name val="IPA Pゴシック"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -96,6 +100,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -169,13 +174,12 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="24.527027027027"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.1711711711712"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="24.4324324324324"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -226,12 +230,12 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -243,7 +247,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>